<commit_message>
Mudanças significativas na interface e comportamento
</commit_message>
<xml_diff>
--- a/data/15-10-2021-FINAL REPORT.xlsx
+++ b/data/15-10-2021-FINAL REPORT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="176">
   <si>
     <t>Number</t>
   </si>
@@ -74,36 +74,213 @@
     <t>DSS - Brazil - Macaé</t>
   </si>
   <si>
+    <t>TASK1509144</t>
+  </si>
+  <si>
+    <t>Robson Silva-External</t>
+  </si>
+  <si>
+    <t>13-10-2021</t>
+  </si>
+  <si>
+    <t>TASK0055542</t>
+  </si>
+  <si>
+    <t>Guilherme Sousa-External</t>
+  </si>
+  <si>
+    <t>DSS - Brazil - Rio de Janeiro / Pavuna</t>
+  </si>
+  <si>
+    <t>27-09-2021</t>
+  </si>
+  <si>
+    <t>14-10-2021</t>
+  </si>
+  <si>
+    <t>TASK1485815</t>
+  </si>
+  <si>
+    <t>Leandro Pereira-External</t>
+  </si>
+  <si>
+    <t>18-08-2021</t>
+  </si>
+  <si>
+    <t>05-10-2021</t>
+  </si>
+  <si>
+    <t>TASK1510120</t>
+  </si>
+  <si>
+    <t>Henry Soares-External</t>
+  </si>
+  <si>
+    <t>07-10-2021</t>
+  </si>
+  <si>
+    <t>TASK1508736</t>
+  </si>
+  <si>
+    <t>TASK1508454</t>
+  </si>
+  <si>
+    <t>TASK1506276</t>
+  </si>
+  <si>
+    <t>Felipe Oliveira-External</t>
+  </si>
+  <si>
+    <t>DSS - Brazil - São João da Barra</t>
+  </si>
+  <si>
+    <t>30-09-2021</t>
+  </si>
+  <si>
+    <t>TASK0055548</t>
+  </si>
+  <si>
+    <t>TASK1506842</t>
+  </si>
+  <si>
+    <t>01-10-2021</t>
+  </si>
+  <si>
+    <t>TASK1509295</t>
+  </si>
+  <si>
+    <t>TASK1509176</t>
+  </si>
+  <si>
+    <t>Euzebio Rodrigues-External</t>
+  </si>
+  <si>
+    <t>TASK1510301</t>
+  </si>
+  <si>
+    <t>TASK1510822</t>
+  </si>
+  <si>
+    <t>TASK1509565</t>
+  </si>
+  <si>
+    <t>TASK0056330</t>
+  </si>
+  <si>
+    <t>TASK1508354</t>
+  </si>
+  <si>
+    <t>TASK0055761</t>
+  </si>
+  <si>
+    <t>Ralphy Messias-External</t>
+  </si>
+  <si>
+    <t>DSS - Brazil - Vitória</t>
+  </si>
+  <si>
+    <t>29-09-2021</t>
+  </si>
+  <si>
+    <t>TASK1508634</t>
+  </si>
+  <si>
+    <t>TASK0056334</t>
+  </si>
+  <si>
+    <t>TASK1508633</t>
+  </si>
+  <si>
+    <t>TASK0056329</t>
+  </si>
+  <si>
+    <t>TASK1509186</t>
+  </si>
+  <si>
+    <t>TASK1505656</t>
+  </si>
+  <si>
+    <t>TASK1507834</t>
+  </si>
+  <si>
+    <t>04-10-2021</t>
+  </si>
+  <si>
+    <t>TASK1506220</t>
+  </si>
+  <si>
+    <t>TASK1508641</t>
+  </si>
+  <si>
+    <t>TASK1509338</t>
+  </si>
+  <si>
+    <t>TASK0056436</t>
+  </si>
+  <si>
+    <t>TASK1509199</t>
+  </si>
+  <si>
+    <t>TASK1509983</t>
+  </si>
+  <si>
+    <t>TASK0056311</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>TASK0056399</t>
+  </si>
+  <si>
+    <t>TASK1508776</t>
+  </si>
+  <si>
+    <t>TASK1510590</t>
+  </si>
+  <si>
+    <t>TASK0055331</t>
+  </si>
+  <si>
+    <t>23-09-2021</t>
+  </si>
+  <si>
+    <t>TASK1509915</t>
+  </si>
+  <si>
+    <t>TASK1507739</t>
+  </si>
+  <si>
+    <t>TASK0056381</t>
+  </si>
+  <si>
+    <t>TASK1510519</t>
+  </si>
+  <si>
+    <t>TASK1507611</t>
+  </si>
+  <si>
+    <t>TASK1506402</t>
+  </si>
+  <si>
+    <t>TASK1507855</t>
+  </si>
+  <si>
+    <t>TASK1510627</t>
+  </si>
+  <si>
+    <t>TASK1508399</t>
+  </si>
+  <si>
     <t>TASK1490438</t>
   </si>
   <si>
-    <t>Leandro Pereira-External</t>
-  </si>
-  <si>
     <t>27-08-2021</t>
   </si>
   <si>
-    <t>05-10-2021</t>
-  </si>
-  <si>
-    <t>TASK1509144</t>
-  </si>
-  <si>
-    <t>Robson Silva-External</t>
-  </si>
-  <si>
-    <t>13-10-2021</t>
-  </si>
-  <si>
     <t>TASK1481727</t>
   </si>
   <si>
-    <t>Euzebio Rodrigues-External</t>
-  </si>
-  <si>
-    <t>DSS - Brazil - Rio de Janeiro / Pavuna</t>
-  </si>
-  <si>
     <t>09-08-2021</t>
   </si>
   <si>
@@ -131,16 +308,10 @@
     <t>26-08-2021</t>
   </si>
   <si>
-    <t>TASK0055542</t>
-  </si>
-  <si>
-    <t>Guilherme Sousa-External</t>
-  </si>
-  <si>
-    <t>27-09-2021</t>
-  </si>
-  <si>
-    <t>14-10-2021</t>
+    <t>TASK0051994</t>
+  </si>
+  <si>
+    <t>02-08-2021</t>
   </si>
   <si>
     <t>TASK1486986</t>
@@ -149,19 +320,7 @@
     <t>20-08-2021</t>
   </si>
   <si>
-    <t>TASK1485815</t>
-  </si>
-  <si>
-    <t>18-08-2021</t>
-  </si>
-  <si>
-    <t>TASK1510120</t>
-  </si>
-  <si>
-    <t>Henry Soares-External</t>
-  </si>
-  <si>
-    <t>07-10-2021</t>
+    <t>15-10-2021</t>
   </si>
   <si>
     <t>TASK1500739</t>
@@ -182,24 +341,6 @@
     <t>16-09-2021</t>
   </si>
   <si>
-    <t>TASK1508736</t>
-  </si>
-  <si>
-    <t>TASK1508454</t>
-  </si>
-  <si>
-    <t>TASK1506276</t>
-  </si>
-  <si>
-    <t>Felipe Oliveira-External</t>
-  </si>
-  <si>
-    <t>DSS - Brazil - São João da Barra</t>
-  </si>
-  <si>
-    <t>30-09-2021</t>
-  </si>
-  <si>
     <t>TASK1485890</t>
   </si>
   <si>
@@ -209,9 +350,6 @@
     <t>21-09-2021</t>
   </si>
   <si>
-    <t>TASK0055548</t>
-  </si>
-  <si>
     <t>TASK1481148</t>
   </si>
   <si>
@@ -245,18 +383,6 @@
     <t>TASK1501314</t>
   </si>
   <si>
-    <t>TASK1506842</t>
-  </si>
-  <si>
-    <t>01-10-2021</t>
-  </si>
-  <si>
-    <t>TASK1509295</t>
-  </si>
-  <si>
-    <t>TASK1509176</t>
-  </si>
-  <si>
     <t>TASK1486604</t>
   </si>
   <si>
@@ -269,9 +395,6 @@
     <t>15-09-2021</t>
   </si>
   <si>
-    <t>TASK1510301</t>
-  </si>
-  <si>
     <t>TASK1498530</t>
   </si>
   <si>
@@ -281,9 +404,6 @@
     <t>24-09-2021</t>
   </si>
   <si>
-    <t>TASK1510822</t>
-  </si>
-  <si>
     <t>TASK1496871</t>
   </si>
   <si>
@@ -296,54 +416,18 @@
     <t>TASK1481392</t>
   </si>
   <si>
-    <t>TASK1509565</t>
-  </si>
-  <si>
-    <t>TASK0056330</t>
-  </si>
-  <si>
     <t>TASK1486444</t>
   </si>
   <si>
-    <t>TASK1508354</t>
-  </si>
-  <si>
     <t>TASK1493927</t>
   </si>
   <si>
     <t>04-09-2021</t>
   </si>
   <si>
-    <t>TASK0055761</t>
-  </si>
-  <si>
-    <t>Ralphy Messias-External</t>
-  </si>
-  <si>
-    <t>DSS - Brazil - Vitória</t>
-  </si>
-  <si>
-    <t>29-09-2021</t>
-  </si>
-  <si>
-    <t>TASK1508634</t>
-  </si>
-  <si>
-    <t>TASK0056334</t>
-  </si>
-  <si>
-    <t>TASK1508633</t>
-  </si>
-  <si>
     <t>TASK1483667</t>
   </si>
   <si>
-    <t>TASK0056329</t>
-  </si>
-  <si>
-    <t>TASK1509186</t>
-  </si>
-  <si>
     <t>TASK1500529</t>
   </si>
   <si>
@@ -353,24 +437,9 @@
     <t>25-08-2021</t>
   </si>
   <si>
-    <t>TASK1505656</t>
-  </si>
-  <si>
-    <t>TASK1507834</t>
-  </si>
-  <si>
-    <t>04-10-2021</t>
-  </si>
-  <si>
     <t>TASK1489121</t>
   </si>
   <si>
-    <t>TASK1506220</t>
-  </si>
-  <si>
-    <t>TASK1508641</t>
-  </si>
-  <si>
     <t>TASK1500369</t>
   </si>
   <si>
@@ -383,15 +452,6 @@
     <t>TASK1500646</t>
   </si>
   <si>
-    <t>TASK1509338</t>
-  </si>
-  <si>
-    <t>TASK0056436</t>
-  </si>
-  <si>
-    <t>TASK1509199</t>
-  </si>
-  <si>
     <t>TASK1496296</t>
   </si>
   <si>
@@ -413,42 +473,18 @@
     <t>TASK1505668</t>
   </si>
   <si>
-    <t>TASK1509983</t>
-  </si>
-  <si>
     <t>TASK1504738</t>
   </si>
   <si>
     <t>28-09-2021</t>
   </si>
   <si>
-    <t>TASK0056311</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>TASK0056399</t>
-  </si>
-  <si>
     <t>TASK1486142</t>
   </si>
   <si>
-    <t>TASK1508776</t>
-  </si>
-  <si>
     <t>TASK1504853</t>
   </si>
   <si>
-    <t>TASK1510590</t>
-  </si>
-  <si>
-    <t>TASK0055331</t>
-  </si>
-  <si>
-    <t>23-09-2021</t>
-  </si>
-  <si>
     <t>TASK1505559</t>
   </si>
   <si>
@@ -458,15 +494,6 @@
     <t>03-09-2021</t>
   </si>
   <si>
-    <t>TASK1509915</t>
-  </si>
-  <si>
-    <t>TASK1507739</t>
-  </si>
-  <si>
-    <t>TASK0056381</t>
-  </si>
-  <si>
     <t>TASK1491710</t>
   </si>
   <si>
@@ -476,21 +503,9 @@
     <t>TASK1502560</t>
   </si>
   <si>
-    <t>TASK1510519</t>
-  </si>
-  <si>
     <t>TASK1482035</t>
   </si>
   <si>
-    <t>TASK1507611</t>
-  </si>
-  <si>
-    <t>TASK1506402</t>
-  </si>
-  <si>
-    <t>TASK1507855</t>
-  </si>
-  <si>
     <t>TASK1484107</t>
   </si>
   <si>
@@ -506,9 +521,6 @@
     <t>16-08-2021</t>
   </si>
   <si>
-    <t>TASK1510627</t>
-  </si>
-  <si>
     <t>TASK1497524</t>
   </si>
   <si>
@@ -522,9 +534,6 @@
   </si>
   <si>
     <t>TASK1502177</t>
-  </si>
-  <si>
-    <t>TASK1508399</t>
   </si>
   <si>
     <t>TASK1502457</t>
@@ -575,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -695,41 +704,41 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -738,67 +747,67 @@
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -806,64 +815,64 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
-      </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -875,55 +884,55 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -935,118 +944,118 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1055,198 +1064,198 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1258,55 +1267,55 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="F36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
@@ -1315,38 +1324,38 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -1355,87 +1364,87 @@
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -1443,130 +1452,130 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="F47" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -1575,38 +1584,38 @@
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F50" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F51" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -1615,38 +1624,38 @@
         <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -1655,18 +1664,18 @@
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="F54" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
@@ -1675,478 +1684,478 @@
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="F55" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="F56" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F57" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="F63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D64" t="s">
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="F64" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B65" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="F65" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
       </c>
       <c r="E67" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="F67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="F68" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="F69" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D70" t="s">
         <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="F70" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
         <v>126</v>
       </c>
-      <c r="B71" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" t="s">
-        <v>127</v>
-      </c>
       <c r="F71" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
       </c>
       <c r="E72" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F72" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
       </c>
       <c r="E73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D74" t="s">
         <v>9</v>
       </c>
       <c r="E74" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F74" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
       </c>
       <c r="E75" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="F75" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B76" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C76" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
       </c>
       <c r="E76" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="F76" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="F77" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="F78" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -2155,18 +2164,18 @@
         <v>9</v>
       </c>
       <c r="E79" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
@@ -2175,230 +2184,230 @@
         <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="F80" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D81" t="s">
         <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="F81" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
         <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="F82" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D83" t="s">
         <v>9</v>
       </c>
       <c r="E83" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F83" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B84" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C84" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D84" t="s">
         <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F84" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
       </c>
       <c r="E85" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
       </c>
       <c r="E86" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="F86" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C87" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D87" t="s">
         <v>9</v>
       </c>
       <c r="E87" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="F87" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="D88" t="s">
         <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="F88" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>150</v>
+      </c>
+      <c r="B89" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="s">
         <v>151</v>
       </c>
-      <c r="B89" t="s">
-        <v>28</v>
-      </c>
-      <c r="C89" t="s">
-        <v>29</v>
-      </c>
-      <c r="D89" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" t="s">
-        <v>152</v>
-      </c>
       <c r="F89" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B90" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C90" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D90" t="s">
         <v>9</v>
       </c>
       <c r="E90" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="F90" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s">
         <v>154</v>
       </c>
-      <c r="B91" t="s">
-        <v>12</v>
-      </c>
-      <c r="C91" t="s">
-        <v>13</v>
-      </c>
-      <c r="D91" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
       <c r="F91" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
@@ -2406,10 +2415,10 @@
         <v>155</v>
       </c>
       <c r="B92" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D92" t="s">
         <v>9</v>
@@ -2418,7 +2427,7 @@
         <v>30</v>
       </c>
       <c r="F92" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93">
@@ -2426,19 +2435,19 @@
         <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D93" t="s">
         <v>9</v>
       </c>
       <c r="E93" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="F93" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
@@ -2446,19 +2455,19 @@
         <v>157</v>
       </c>
       <c r="B94" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C94" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="D94" t="s">
         <v>9</v>
       </c>
       <c r="E94" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F94" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95">
@@ -2466,7 +2475,7 @@
         <v>158</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -2475,70 +2484,70 @@
         <v>9</v>
       </c>
       <c r="E95" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="F95" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D96" t="s">
         <v>9</v>
       </c>
       <c r="E96" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F96" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C97" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D97" t="s">
         <v>9</v>
       </c>
       <c r="E97" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="F97" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
       </c>
       <c r="E98" t="s">
-        <v>163</v>
+        <v>89</v>
       </c>
       <c r="F98" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99">
@@ -2546,7 +2555,7 @@
         <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -2555,30 +2564,30 @@
         <v>9</v>
       </c>
       <c r="E99" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="F99" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
       </c>
       <c r="E100" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="F100" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101">
@@ -2586,10 +2595,10 @@
         <v>167</v>
       </c>
       <c r="B101" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -2598,7 +2607,7 @@
         <v>168</v>
       </c>
       <c r="F101" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102">
@@ -2606,79 +2615,1059 @@
         <v>169</v>
       </c>
       <c r="B102" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C102" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D102" t="s">
         <v>9</v>
       </c>
       <c r="E102" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F102" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D103" t="s">
         <v>9</v>
       </c>
       <c r="E103" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="F103" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C104" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D104" t="s">
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="F104" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B105" t="s">
+        <v>46</v>
+      </c>
+      <c r="C105" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" t="s">
+        <v>76</v>
+      </c>
+      <c r="F105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>175</v>
+      </c>
+      <c r="B106" t="s">
+        <v>46</v>
+      </c>
+      <c r="C106" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" t="s">
+        <v>111</v>
+      </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" t="s">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" t="s">
+        <v>13</v>
+      </c>
+      <c r="D109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>17</v>
+      </c>
+      <c r="B110" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
         <v>28</v>
       </c>
-      <c r="C105" t="s">
+      <c r="B113" t="s">
         <v>29</v>
       </c>
-      <c r="D105" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" t="s">
+        <v>30</v>
+      </c>
+      <c r="F113" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C114" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" t="s">
+        <v>34</v>
+      </c>
+      <c r="F114" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" t="s">
+        <v>31</v>
+      </c>
+      <c r="F115" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>36</v>
+      </c>
+      <c r="B116" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" t="s">
+        <v>19</v>
+      </c>
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" t="s">
+        <v>31</v>
+      </c>
+      <c r="F116" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>37</v>
+      </c>
+      <c r="B117" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" t="s">
+        <v>40</v>
+      </c>
+      <c r="F117" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>41</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" t="s">
+        <v>26</v>
+      </c>
+      <c r="F118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>42</v>
+      </c>
+      <c r="B119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" t="s">
+        <v>43</v>
+      </c>
+      <c r="F119" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>44</v>
+      </c>
+      <c r="B120" t="s">
+        <v>21</v>
+      </c>
+      <c r="C120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>45</v>
+      </c>
+      <c r="B121" t="s">
+        <v>46</v>
+      </c>
+      <c r="C121" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>47</v>
+      </c>
+      <c r="B122" t="s">
+        <v>18</v>
+      </c>
+      <c r="C122" t="s">
+        <v>19</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" t="s">
+        <v>34</v>
+      </c>
+      <c r="F122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>48</v>
+      </c>
+      <c r="B123" t="s">
+        <v>21</v>
+      </c>
+      <c r="C123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>49</v>
+      </c>
+      <c r="B124" t="s">
+        <v>46</v>
+      </c>
+      <c r="C124" t="s">
+        <v>25</v>
+      </c>
+      <c r="D124" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>50</v>
+      </c>
+      <c r="B125" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" t="s">
+        <v>34</v>
+      </c>
+      <c r="F125" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>51</v>
+      </c>
+      <c r="B126" t="s">
+        <v>46</v>
+      </c>
+      <c r="C126" t="s">
+        <v>25</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
+        <v>31</v>
+      </c>
+      <c r="F126" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>52</v>
+      </c>
+      <c r="B127" t="s">
+        <v>53</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" t="s">
+        <v>55</v>
+      </c>
+      <c r="F127" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>56</v>
+      </c>
+      <c r="B128" t="s">
+        <v>29</v>
+      </c>
+      <c r="C128" t="s">
+        <v>8</v>
+      </c>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" t="s">
+        <v>31</v>
+      </c>
+      <c r="F128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>57</v>
+      </c>
+      <c r="B129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" t="s">
+        <v>34</v>
+      </c>
+      <c r="F129" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>58</v>
+      </c>
+      <c r="B130" t="s">
+        <v>21</v>
+      </c>
+      <c r="C130" t="s">
+        <v>8</v>
+      </c>
+      <c r="D130" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" t="s">
+        <v>31</v>
+      </c>
+      <c r="F130" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>59</v>
+      </c>
+      <c r="B131" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" t="s">
+        <v>34</v>
+      </c>
+      <c r="F131" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>60</v>
+      </c>
+      <c r="B132" t="s">
+        <v>46</v>
+      </c>
+      <c r="C132" t="s">
+        <v>25</v>
+      </c>
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" t="s">
+        <v>10</v>
+      </c>
+      <c r="F132" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>61</v>
+      </c>
+      <c r="B133" t="s">
+        <v>46</v>
+      </c>
+      <c r="C133" t="s">
+        <v>25</v>
+      </c>
+      <c r="D133" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" t="s">
+        <v>55</v>
+      </c>
+      <c r="F133" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>62</v>
+      </c>
+      <c r="B134" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" t="s">
+        <v>8</v>
+      </c>
+      <c r="D134" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" t="s">
+        <v>63</v>
+      </c>
+      <c r="F134" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
         <v>64</v>
       </c>
-      <c r="F105" t="s">
-        <v>26</v>
+      <c r="B135" t="s">
+        <v>29</v>
+      </c>
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" t="s">
+        <v>40</v>
+      </c>
+      <c r="F135" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>65</v>
+      </c>
+      <c r="B136" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" t="s">
+        <v>31</v>
+      </c>
+      <c r="F136" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>66</v>
+      </c>
+      <c r="B137" t="s">
+        <v>46</v>
+      </c>
+      <c r="C137" t="s">
+        <v>25</v>
+      </c>
+      <c r="D137" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>67</v>
+      </c>
+      <c r="B138" t="s">
+        <v>33</v>
+      </c>
+      <c r="C138" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>68</v>
+      </c>
+      <c r="B139" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>69</v>
+      </c>
+      <c r="B140" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" t="s">
+        <v>8</v>
+      </c>
+      <c r="D140" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" t="s">
+        <v>34</v>
+      </c>
+      <c r="F140" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>70</v>
+      </c>
+      <c r="B141" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" t="s">
+        <v>13</v>
+      </c>
+      <c r="D141" t="s">
+        <v>71</v>
+      </c>
+      <c r="E141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F141" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>72</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" t="s">
+        <v>9</v>
+      </c>
+      <c r="E142" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>73</v>
+      </c>
+      <c r="B143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
+        <v>9</v>
+      </c>
+      <c r="E143" t="s">
+        <v>31</v>
+      </c>
+      <c r="F143" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>74</v>
+      </c>
+      <c r="B144" t="s">
+        <v>29</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>9</v>
+      </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>75</v>
+      </c>
+      <c r="B145" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" t="s">
+        <v>9</v>
+      </c>
+      <c r="E145" t="s">
+        <v>76</v>
+      </c>
+      <c r="F145" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>77</v>
+      </c>
+      <c r="B146" t="s">
+        <v>46</v>
+      </c>
+      <c r="C146" t="s">
+        <v>25</v>
+      </c>
+      <c r="D146" t="s">
+        <v>9</v>
+      </c>
+      <c r="E146" t="s">
+        <v>34</v>
+      </c>
+      <c r="F146" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>78</v>
+      </c>
+      <c r="B147" t="s">
+        <v>33</v>
+      </c>
+      <c r="C147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" t="s">
+        <v>9</v>
+      </c>
+      <c r="E147" t="s">
+        <v>63</v>
+      </c>
+      <c r="F147" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>79</v>
+      </c>
+      <c r="B148" t="s">
+        <v>53</v>
+      </c>
+      <c r="C148" t="s">
+        <v>54</v>
+      </c>
+      <c r="D148" t="s">
+        <v>9</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" t="s">
+        <v>9</v>
+      </c>
+      <c r="E149" t="s">
+        <v>14</v>
+      </c>
+      <c r="F149" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>81</v>
+      </c>
+      <c r="B150" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" t="s">
+        <v>9</v>
+      </c>
+      <c r="E150" t="s">
+        <v>63</v>
+      </c>
+      <c r="F150" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>82</v>
+      </c>
+      <c r="B151" t="s">
+        <v>38</v>
+      </c>
+      <c r="C151" t="s">
+        <v>39</v>
+      </c>
+      <c r="D151" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151" t="s">
+        <v>40</v>
+      </c>
+      <c r="F151" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>83</v>
+      </c>
+      <c r="B152" t="s">
+        <v>21</v>
+      </c>
+      <c r="C152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" t="s">
+        <v>63</v>
+      </c>
+      <c r="F152" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>84</v>
+      </c>
+      <c r="B153" t="s">
+        <v>29</v>
+      </c>
+      <c r="C153" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" t="s">
+        <v>14</v>
+      </c>
+      <c r="F153" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>85</v>
+      </c>
+      <c r="B154" t="s">
+        <v>21</v>
+      </c>
+      <c r="C154" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" t="s">
+        <v>9</v>
+      </c>
+      <c r="E154" t="s">
+        <v>31</v>
+      </c>
+      <c r="F154" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>